<commit_message>
dataprovider class and implementation is created
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/testdata.xlsx
+++ b/src/test/resources/ExcelFiles/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamal\eclipse-workspace\OrangeHrm\src\test\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93E77B5D-8EC6-48B6-94BF-C299E1A67AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D6AACE-AE2C-4171-B414-5DA96AF5649D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{6F73421B-B79C-4BC2-8D26-BBA593FDEA5A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Username</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Hello</t>
+  </si>
+  <si>
+    <t>Qedge123!@#</t>
   </si>
 </sst>
 </file>
@@ -394,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C11A418-82F2-45F5-BD50-E9507C63424C}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,20 +423,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change the login in datacenter frame
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/testdata.xlsx
+++ b/src/test/resources/ExcelFiles/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamal\eclipse-workspace\OrangeHrm\src\test\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D6AACE-AE2C-4171-B414-5DA96AF5649D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D729F9-E8B0-4561-9458-1860B8A7CCF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{6F73421B-B79C-4BC2-8D26-BBA593FDEA5A}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLoginDetails" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -46,6 +47,18 @@
   </si>
   <si>
     <t>Qedge123!@#</t>
+  </si>
+  <si>
+    <t>Password cannot be empty</t>
+  </si>
+  <si>
+    <t>ErrorMessage</t>
+  </si>
+  <si>
+    <t>Username cannot be empty</t>
+  </si>
+  <si>
+    <t>Invalid credentials</t>
   </si>
 </sst>
 </file>
@@ -397,10 +410,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C11A418-82F2-45F5-BD50-E9507C63424C}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5780EB-956E-4DC3-95EF-65B449836B86}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,34 +499,8 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>